<commit_message>
Přidána hodnotící tabulka do diplomky Přidány nové screenschoty Přidána aplikace Clarity Dodělány citace
</commit_message>
<xml_diff>
--- a/Grafy a schemata/Srovnávací tabulka aplikací.xlsx
+++ b/Grafy a schemata/Srovnávací tabulka aplikací.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="24">
   <si>
     <t>Název aplikace</t>
   </si>
@@ -22,9 +22,6 @@
     <t>Typ</t>
   </si>
   <si>
-    <t>Počet fukcí (modulů)</t>
-  </si>
-  <si>
     <t>Responzivní design</t>
   </si>
   <si>
@@ -52,13 +49,43 @@
     <t>SiDiary</t>
   </si>
   <si>
-    <t>Zápis deníku</t>
-  </si>
-  <si>
     <t>Počet sledovaných parametrů (variabilita)</t>
   </si>
   <si>
     <t>Nightscout</t>
+  </si>
+  <si>
+    <t>Ne</t>
+  </si>
+  <si>
+    <t>Ano</t>
+  </si>
+  <si>
+    <t>Počítačová aplikace</t>
+  </si>
+  <si>
+    <t>Webová aplikace</t>
+  </si>
+  <si>
+    <t>Dexcom Clarity</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Možnost přepnutí měřených jednotek</t>
+  </si>
+  <si>
+    <t>Zápis diabetického deníku</t>
+  </si>
+  <si>
+    <t>Počet funkcí (modulů)</t>
+  </si>
+  <si>
+    <t>Česká lokalizace</t>
+  </si>
+  <si>
+    <t>Ano (statistiky Ne)</t>
   </si>
 </sst>
 </file>
@@ -97,14 +124,16 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -410,81 +439,312 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="11.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" style="1" customWidth="1"/>
-    <col min="8" max="9" width="11.140625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="22.28515625" style="1" customWidth="1"/>
-    <col min="11" max="13" width="11.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="11.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" style="4" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="13" style="4" customWidth="1"/>
+    <col min="10" max="10" width="19.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="17.42578125" style="4" customWidth="1"/>
+    <col min="12" max="13" width="11.140625" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:14" s="2" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="I1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4">
+        <v>9</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="4">
+        <v>1</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L3" s="4">
+        <v>1</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N3" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="4">
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="4">
+        <v>4</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N4" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="4">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="D5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L5" s="3">
         <v>4</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="M5" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="4">
+        <v>8</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="4">
+        <v>9</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L7" s="4">
+        <v>1</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="N7" s="4" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>